<commit_message>
Added Layouts for remaining site data. Added soil moisture sensors. Can now enter data for Glacier and Gribble gap. TODO: Add well layouts for CC and LB
</commit_message>
<xml_diff>
--- a/src/edu/wcu/wchrs/groundwater/files/rounds.xlsx
+++ b/src/edu/wcu/wchrs/groundwater/files/rounds.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="266">
   <si>
     <t>Level:</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -841,6 +841,30 @@
   </si>
   <si>
     <t>GGDistStaff</t>
+  </si>
+  <si>
+    <t>gSMA</t>
+  </si>
+  <si>
+    <t>gSMB</t>
+  </si>
+  <si>
+    <t>gSMC</t>
+  </si>
+  <si>
+    <t>wSMA</t>
+  </si>
+  <si>
+    <t>wSMB</t>
+  </si>
+  <si>
+    <t>wSMC</t>
+  </si>
+  <si>
+    <t>ggSMR</t>
+  </si>
+  <si>
+    <t>ggSML</t>
   </si>
 </sst>
 </file>
@@ -1445,8 +1469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R102"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -1815,6 +1839,9 @@
       <c r="K12" t="s">
         <v>87</v>
       </c>
+      <c r="L12" t="s">
+        <v>264</v>
+      </c>
       <c r="M12" s="37" t="s">
         <v>101</v>
       </c>
@@ -1854,6 +1881,9 @@
       <c r="H13" s="36"/>
       <c r="K13" t="s">
         <v>88</v>
+      </c>
+      <c r="L13" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.2">
@@ -2179,6 +2209,9 @@
       <c r="K25" s="8" t="s">
         <v>90</v>
       </c>
+      <c r="L25" s="8" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
@@ -2203,6 +2236,9 @@
       <c r="K26" s="8" t="s">
         <v>91</v>
       </c>
+      <c r="L26" s="8" t="s">
+        <v>262</v>
+      </c>
       <c r="M26" s="8" t="s">
         <v>106</v>
       </c>
@@ -2227,6 +2263,9 @@
       <c r="J27" s="2"/>
       <c r="K27" s="37" t="s">
         <v>92</v>
+      </c>
+      <c r="L27" t="s">
+        <v>263</v>
       </c>
       <c r="M27" s="8" t="s">
         <v>107</v>
@@ -2348,7 +2387,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="33" spans="2:11" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:12" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B33" s="30"/>
       <c r="C33" s="30"/>
       <c r="D33" s="20"/>
@@ -2367,7 +2406,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>17</v>
       </c>
@@ -2396,7 +2435,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>35</v>
       </c>
@@ -2422,7 +2461,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>36</v>
       </c>
@@ -2449,8 +2488,11 @@
       <c r="K36" s="8" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L36" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>18</v>
       </c>
@@ -2473,8 +2515,11 @@
       <c r="K37" s="8" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L37" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>19</v>
       </c>
@@ -2491,8 +2536,11 @@
       <c r="K38" s="37" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="39" spans="2:11" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="L38" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" ht="16.2" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>20</v>
       </c>
@@ -2510,7 +2558,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>37</v>
       </c>
@@ -2535,7 +2583,7 @@
       </c>
       <c r="K40" s="45"/>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>21</v>
       </c>
@@ -2562,7 +2610,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>38</v>
       </c>
@@ -2589,7 +2637,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>39</v>
       </c>
@@ -2616,7 +2664,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>23</v>
       </c>
@@ -2643,7 +2691,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>40</v>
       </c>
@@ -2664,7 +2712,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>41</v>
       </c>
@@ -2688,7 +2736,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>24</v>
       </c>
@@ -2706,7 +2754,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Added Wind. TODO: Add well layouts for LB/CC, Update LB Controller, and add CC
</commit_message>
<xml_diff>
--- a/src/edu/wcu/wchrs/groundwater/files/rounds.xlsx
+++ b/src/edu/wcu/wchrs/groundwater/files/rounds.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="269">
   <si>
     <t>Level:</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -534,9 +534,6 @@
     <t>WindSlopeDepth</t>
   </si>
   <si>
-    <t>WindCulvert</t>
-  </si>
-  <si>
     <t>GlacierArrivTime</t>
   </si>
   <si>
@@ -865,6 +862,18 @@
   </si>
   <si>
     <t>ggSML</t>
+  </si>
+  <si>
+    <t>WindCulvert1</t>
+  </si>
+  <si>
+    <t>WindCulvertAvg</t>
+  </si>
+  <si>
+    <t>WindCulvert3</t>
+  </si>
+  <si>
+    <t>WindCulvert2</t>
   </si>
 </sst>
 </file>
@@ -1470,7 +1479,7 @@
   <dimension ref="A1:R102"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -1506,19 +1515,19 @@
         <v>77</v>
       </c>
       <c r="H1" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="I1" s="36" t="s">
         <v>244</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="J1" s="36" t="s">
         <v>245</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="K1" s="36" t="s">
         <v>246</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="L1" s="36" t="s">
         <v>247</v>
-      </c>
-      <c r="L1" s="36" t="s">
-        <v>248</v>
       </c>
       <c r="M1" s="38" t="s">
         <v>97</v>
@@ -1572,7 +1581,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20" t="s">
@@ -1589,7 +1598,7 @@
         <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D5" s="20">
         <v>3.3319999999999999</v>
@@ -1622,7 +1631,7 @@
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="41" t="s">
@@ -1641,28 +1650,28 @@
         <v>0</v>
       </c>
       <c r="K6" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="L6" s="35" t="s">
         <v>249</v>
-      </c>
-      <c r="L6" s="35" t="s">
-        <v>250</v>
       </c>
       <c r="M6" s="37" t="s">
         <v>101</v>
       </c>
       <c r="N6" s="37" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O6" s="8" t="s">
         <v>100</v>
       </c>
       <c r="P6" s="37" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Q6" s="8" t="s">
         <v>103</v>
       </c>
       <c r="R6" s="37" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.2">
@@ -1670,7 +1679,7 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="20" t="s">
@@ -1689,10 +1698,10 @@
         <v>4</v>
       </c>
       <c r="K7" s="42" t="s">
+        <v>250</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
@@ -1708,16 +1717,16 @@
         <v>45</v>
       </c>
       <c r="H8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="K8" s="42" t="s">
+        <v>252</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>254</v>
       </c>
       <c r="M8" s="39" t="s">
         <v>102</v>
@@ -1728,7 +1737,7 @@
         <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="41" t="s">
@@ -1747,28 +1756,28 @@
         <v>3</v>
       </c>
       <c r="K9" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="L9" s="7" t="s">
         <v>255</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>256</v>
       </c>
       <c r="M9" s="37" t="s">
         <v>101</v>
       </c>
       <c r="N9" s="37" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O9" s="8" t="s">
         <v>100</v>
       </c>
       <c r="P9" s="37" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="Q9" s="8" t="s">
         <v>103</v>
       </c>
       <c r="R9" s="37" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.2">
@@ -1776,7 +1785,7 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="41" t="s">
@@ -1801,7 +1810,7 @@
         <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="41" t="s">
@@ -1827,7 +1836,7 @@
         <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="41" t="s">
@@ -1840,25 +1849,25 @@
         <v>87</v>
       </c>
       <c r="L12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="M12" s="37" t="s">
         <v>101</v>
       </c>
       <c r="N12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="O12" s="8" t="s">
         <v>100</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="Q12" s="8" t="s">
         <v>103</v>
       </c>
       <c r="R12" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.2">
@@ -1866,7 +1875,7 @@
         <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="41" t="s">
@@ -1883,7 +1892,7 @@
         <v>88</v>
       </c>
       <c r="L13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.2">
@@ -1891,7 +1900,7 @@
         <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="41" t="s">
@@ -1912,7 +1921,7 @@
         <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="41" t="s">
@@ -1925,19 +1934,19 @@
         <v>101</v>
       </c>
       <c r="N15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O15" s="8" t="s">
         <v>100</v>
       </c>
       <c r="P15" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="Q15" s="8" t="s">
         <v>103</v>
       </c>
       <c r="R15" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="2:18" ht="16.2" x14ac:dyDescent="0.3">
@@ -1945,7 +1954,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="41" t="s">
@@ -1963,7 +1972,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="41" t="s">
@@ -1995,25 +2004,25 @@
         <v>2</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M18" s="8" t="s">
         <v>101</v>
       </c>
       <c r="N18" s="37" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O18" s="8" t="s">
         <v>100</v>
       </c>
       <c r="P18" s="37" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q18" s="8" t="s">
         <v>103</v>
       </c>
       <c r="R18" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="2:18" ht="16.8" x14ac:dyDescent="0.3">
@@ -2032,7 +2041,7 @@
         <v>48</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.2">
@@ -2040,7 +2049,7 @@
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="41" t="s">
@@ -2066,7 +2075,7 @@
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="41" t="s">
@@ -2085,25 +2094,25 @@
         <v>49</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M21" s="8" t="s">
         <v>101</v>
       </c>
       <c r="N21" s="37" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O21" s="8" t="s">
         <v>100</v>
       </c>
       <c r="P21" s="37" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q21" s="8" t="s">
         <v>103</v>
       </c>
       <c r="R21" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.2">
@@ -2111,7 +2120,7 @@
         <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="41" t="s">
@@ -2130,7 +2139,7 @@
         <v>50</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.2">
@@ -2138,7 +2147,7 @@
         <v>68</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="41" t="s">
@@ -2159,7 +2168,7 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="41" t="s">
@@ -2190,7 +2199,7 @@
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="41" t="s">
@@ -2210,7 +2219,7 @@
         <v>90</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.2">
@@ -2218,7 +2227,7 @@
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="41" t="s">
@@ -2230,20 +2239,17 @@
       <c r="G26" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="H26" t="s">
-        <v>155</v>
-      </c>
       <c r="K26" s="8" t="s">
         <v>91</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M26" s="8" t="s">
         <v>106</v>
       </c>
       <c r="N26" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.2">
@@ -2251,7 +2257,7 @@
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="41" t="s">
@@ -2260,18 +2266,29 @@
       <c r="F27" s="27">
         <v>4.125</v>
       </c>
-      <c r="J27" s="2"/>
+      <c r="G27" t="s">
+        <v>265</v>
+      </c>
+      <c r="H27" t="s">
+        <v>268</v>
+      </c>
+      <c r="I27" t="s">
+        <v>267</v>
+      </c>
+      <c r="J27" t="s">
+        <v>266</v>
+      </c>
       <c r="K27" s="37" t="s">
         <v>92</v>
       </c>
       <c r="L27" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="M27" s="8" t="s">
         <v>107</v>
       </c>
       <c r="N27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="28" spans="2:18" ht="16.2" x14ac:dyDescent="0.3">
@@ -2279,7 +2296,7 @@
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="41" t="s">
@@ -2296,7 +2313,7 @@
         <v>108</v>
       </c>
       <c r="N28" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" spans="2:18" ht="16.2" x14ac:dyDescent="0.3">
@@ -2304,7 +2321,7 @@
         <v>69</v>
       </c>
       <c r="C29" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="41" t="s">
@@ -2321,7 +2338,7 @@
         <v>70</v>
       </c>
       <c r="C30" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D30" s="20">
         <v>3.3010000000000002</v>
@@ -2336,7 +2353,7 @@
         <v>61</v>
       </c>
       <c r="H30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J30" s="44" t="s">
         <v>56</v>
@@ -2348,7 +2365,7 @@
         <v>71</v>
       </c>
       <c r="C31" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D31" s="20"/>
       <c r="E31" s="41" t="s">
@@ -2361,13 +2378,13 @@
         <v>62</v>
       </c>
       <c r="H31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>0</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.2">
@@ -2378,13 +2395,13 @@
         <v>63</v>
       </c>
       <c r="H32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J32" s="13" t="s">
         <v>52</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="33" spans="2:12" ht="16.8" x14ac:dyDescent="0.3">
@@ -2397,13 +2414,13 @@
         <v>45</v>
       </c>
       <c r="H33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J33" s="13" t="s">
         <v>53</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.2">
@@ -2411,7 +2428,7 @@
         <v>17</v>
       </c>
       <c r="C34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D34" s="20">
         <v>3.367</v>
@@ -2426,13 +2443,13 @@
         <v>60</v>
       </c>
       <c r="H34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J34" s="15" t="s">
         <v>50</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.2">
@@ -2440,7 +2457,7 @@
         <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D35" s="20">
         <v>3.5049999999999999</v>
@@ -2455,7 +2472,7 @@
         <v>65</v>
       </c>
       <c r="H35" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K35" s="36" t="s">
         <v>93</v>
@@ -2466,7 +2483,7 @@
         <v>36</v>
       </c>
       <c r="C36" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D36" s="24"/>
       <c r="E36" s="41" t="s">
@@ -2479,7 +2496,7 @@
         <v>81</v>
       </c>
       <c r="H36" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I36" t="s">
         <v>75</v>
@@ -2489,7 +2506,7 @@
         <v>94</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.2">
@@ -2497,7 +2514,7 @@
         <v>18</v>
       </c>
       <c r="C37" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D37" s="20">
         <v>3.3140000000000001</v>
@@ -2516,7 +2533,7 @@
         <v>95</v>
       </c>
       <c r="L37" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.2">
@@ -2524,7 +2541,7 @@
         <v>19</v>
       </c>
       <c r="C38" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D38" s="20"/>
       <c r="E38" s="41" t="s">
@@ -2537,7 +2554,7 @@
         <v>96</v>
       </c>
       <c r="L38" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="39" spans="2:12" ht="16.2" x14ac:dyDescent="0.3">
@@ -2545,7 +2562,7 @@
         <v>20</v>
       </c>
       <c r="C39" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="41" t="s">
@@ -2563,7 +2580,7 @@
         <v>37</v>
       </c>
       <c r="C40" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D40" s="20"/>
       <c r="E40" s="41" t="s">
@@ -2576,7 +2593,7 @@
         <v>61</v>
       </c>
       <c r="H40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J40" s="44" t="s">
         <v>55</v>
@@ -2588,7 +2605,7 @@
         <v>21</v>
       </c>
       <c r="C41" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D41" s="20"/>
       <c r="E41" s="41" t="s">
@@ -2601,13 +2618,13 @@
         <v>62</v>
       </c>
       <c r="H41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J41" s="5" t="s">
         <v>1</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.2">
@@ -2615,7 +2632,7 @@
         <v>38</v>
       </c>
       <c r="C42" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="41" t="s">
@@ -2628,13 +2645,13 @@
         <v>63</v>
       </c>
       <c r="H42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J42" s="5" t="s">
         <v>4</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.2">
@@ -2642,7 +2659,7 @@
         <v>39</v>
       </c>
       <c r="C43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="41" t="s">
@@ -2655,13 +2672,13 @@
         <v>45</v>
       </c>
       <c r="H43" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J43" s="5" t="s">
         <v>5</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.2">
@@ -2669,7 +2686,7 @@
         <v>23</v>
       </c>
       <c r="C44" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="41" t="s">
@@ -2682,13 +2699,13 @@
         <v>64</v>
       </c>
       <c r="H44" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J44" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K44" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.2">
@@ -2696,7 +2713,7 @@
         <v>40</v>
       </c>
       <c r="C45" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="41" t="s">
@@ -2709,7 +2726,7 @@
         <v>60</v>
       </c>
       <c r="H45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.2">
@@ -2717,7 +2734,7 @@
         <v>41</v>
       </c>
       <c r="C46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="41" t="s">
@@ -2730,7 +2747,7 @@
         <v>79</v>
       </c>
       <c r="H46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I46" t="s">
         <v>75</v>
@@ -2741,7 +2758,7 @@
         <v>24</v>
       </c>
       <c r="C47" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="41" t="s">
@@ -2759,7 +2776,7 @@
         <v>42</v>
       </c>
       <c r="C48" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="41" t="s">
@@ -2774,7 +2791,7 @@
         <v>16</v>
       </c>
       <c r="C49" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="41" t="s">

</xml_diff>

<commit_message>
Finished rounds, need to field test. Todo: Add Branding
</commit_message>
<xml_diff>
--- a/src/edu/wcu/wchrs/groundwater/files/rounds.xlsx
+++ b/src/edu/wcu/wchrs/groundwater/files/rounds.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="266">
   <si>
     <t>Level:</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -34,10 +34,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Level:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Notes:</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -234,9 +230,6 @@
     <t>Long Branch</t>
   </si>
   <si>
-    <t>Long Branch Rain Gauge</t>
-  </si>
-  <si>
     <t>Glacier Rain Gauge</t>
   </si>
   <si>
@@ -309,9 +302,6 @@
     <t>LB2streamside</t>
   </si>
   <si>
-    <t>Triple Junction</t>
-  </si>
-  <si>
     <t>Glacier1Well</t>
   </si>
   <si>
@@ -573,9 +563,6 @@
     <t>LBStage</t>
   </si>
   <si>
-    <t>LB2StreamsideDepth</t>
-  </si>
-  <si>
     <t>WindRGLevel</t>
   </si>
   <si>
@@ -600,18 +587,6 @@
     <t>GlacierRGNotes</t>
   </si>
   <si>
-    <t>LBRGLevel</t>
-  </si>
-  <si>
-    <t>LBRGCond</t>
-  </si>
-  <si>
-    <t>LBRGBatt</t>
-  </si>
-  <si>
-    <t>LBRGNotes</t>
-  </si>
-  <si>
     <t>GG1MPTemp</t>
   </si>
   <si>
@@ -723,9 +698,6 @@
     <t>LB3DDepth</t>
   </si>
   <si>
-    <t>LB1strmsideDepth</t>
-  </si>
-  <si>
     <t>LB2SDepth</t>
   </si>
   <si>
@@ -874,6 +846,24 @@
   </si>
   <si>
     <t>WindCulvert2</t>
+  </si>
+  <si>
+    <t>LB1StreamDepth</t>
+  </si>
+  <si>
+    <t>LB2StreamDepth</t>
+  </si>
+  <si>
+    <t>Well Site Notes:</t>
+  </si>
+  <si>
+    <t>CCWellNotes</t>
+  </si>
+  <si>
+    <t>LBWellNotes</t>
+  </si>
+  <si>
+    <t>GGWellNotes</t>
   </si>
 </sst>
 </file>
@@ -1051,7 +1041,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1142,6 +1132,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1478,8 +1472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R102"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -1501,47 +1495,47 @@
   <sheetData>
     <row r="1" spans="2:18" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="16" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E1" s="46"/>
       <c r="F1" s="46"/>
       <c r="G1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H1" s="36" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="I1" s="36" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="J1" s="36" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="K1" s="36" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="L1" s="36" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="M1" s="38" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="25"/>
@@ -1550,26 +1544,26 @@
     </row>
     <row r="3" spans="2:18" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>44</v>
-      </c>
       <c r="G3" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H3" s="10"/>
       <c r="M3" s="43" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="N3" s="43"/>
       <c r="O3" s="43"/>
@@ -1578,14 +1572,14 @@
     </row>
     <row r="4" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F4" s="27">
         <v>3.39</v>
@@ -1595,434 +1589,440 @@
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="D5" s="20">
         <v>3.3319999999999999</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F5" s="27">
         <v>5.3920000000000003</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="J5" s="44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K5" s="47"/>
       <c r="L5" s="34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M5" s="39" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="41" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F6" s="27">
         <v>8.49</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>0</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="L6" s="35" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="M6" s="37" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="N6" s="37" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="O6" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="P6" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q6" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="P6" s="37" t="s">
-        <v>182</v>
-      </c>
-      <c r="Q6" s="8" t="s">
-        <v>103</v>
-      </c>
       <c r="R6" s="37" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="20" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F7" s="27">
         <v>8.1549999999999994</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K7" s="42" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="20" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F8"/>
       <c r="G8" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H8" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K8" s="42" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="M8" s="39" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="41" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F9" s="27">
         <v>3.66</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="M9" s="37" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="N9" s="37" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="O9" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="P9" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q9" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="P9" s="37" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q9" s="8" t="s">
-        <v>103</v>
-      </c>
       <c r="R9" s="37" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="41" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F10" s="27">
         <v>5.24</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H10" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="41" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F11" s="27">
         <v>7.29</v>
       </c>
       <c r="G11" s="8"/>
       <c r="I11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="36" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="M11" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="41" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F12" s="27">
         <v>4.0549999999999997</v>
       </c>
       <c r="K12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="L12" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="M12" s="37" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="N12" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O12" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="P12" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q12" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="P12" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q12" s="8" t="s">
-        <v>103</v>
-      </c>
       <c r="R12" s="8" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="41" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F13" s="27">
         <v>5.36</v>
       </c>
       <c r="G13" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H13" s="36"/>
       <c r="K13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="L13" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="41" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F14" s="27">
         <v>8.5269999999999992</v>
       </c>
       <c r="G14" s="36" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="M14" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="41" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F15" s="27">
         <v>3.69</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="N15" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="O15" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="P15" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q15" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="P15" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q15" s="8" t="s">
-        <v>103</v>
-      </c>
       <c r="R15" s="8" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="2:18" ht="16.2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="41" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F16" s="27">
         <v>5.5549999999999997</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="2:18" ht="16.2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="41" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F17" s="27">
         <v>8.7750000000000004</v>
       </c>
       <c r="G17" s="12"/>
       <c r="J17" s="44" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K17" s="45"/>
       <c r="M17" s="39" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>262</v>
+      </c>
+      <c r="C18" t="s">
+        <v>265</v>
+      </c>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
       <c r="F18" s="27"/>
       <c r="G18" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H18" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="N18" s="37" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="O18" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="P18" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q18" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="P18" s="37" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q18" s="8" t="s">
-        <v>103</v>
-      </c>
       <c r="R18" s="8" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="2:18" ht="16.8" x14ac:dyDescent="0.3">
@@ -2032,300 +2032,300 @@
       <c r="E19" s="20"/>
       <c r="F19"/>
       <c r="G19" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H19" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="41" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F20" s="27">
         <v>3.625</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H20" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="J20" s="13"/>
       <c r="K20" s="1"/>
       <c r="M20" s="39" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="41" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F21" s="27">
         <v>4.8899999999999997</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H21" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="M21" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="N21" s="37" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="O21" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="P21" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q21" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="P21" s="37" t="s">
-        <v>197</v>
-      </c>
-      <c r="Q21" s="8" t="s">
-        <v>103</v>
-      </c>
       <c r="R21" s="8" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="41" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F22" s="27">
         <v>6.44</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H22" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B23" s="31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>218</v>
+        <v>260</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="41" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F23" s="27">
         <v>0.45700000000000002</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H23" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="41" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F24" s="27">
         <v>4.6849999999999996</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H24" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="I24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J24" s="2"/>
       <c r="K24" s="36" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="M24" s="40" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="41" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F25" s="27">
         <v>3.2250000000000001</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="41" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F26" s="27">
         <v>4.34</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="M26" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N26" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="41" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F27" s="27">
         <v>4.125</v>
       </c>
       <c r="G27" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="H27" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="I27" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="J27" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="K27" s="37" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L27" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="M27" s="8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="N27" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="2:18" ht="16.2" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="41" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F28" s="27">
         <v>3.91</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J28" s="2"/>
       <c r="M28" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="N28" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" spans="2:18" ht="16.2" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C29" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="41" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F29" s="27">
         <v>3.42</v>
@@ -2335,73 +2335,79 @@
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C30" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D30" s="20">
         <v>3.3010000000000002</v>
       </c>
       <c r="E30" s="41" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F30" s="27">
         <v>4.87</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H30" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="J30" s="44" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K30" s="45"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C31" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="D31" s="20"/>
       <c r="E31" s="41" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F31" s="27">
         <v>6.61</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H31" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>0</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>262</v>
+      </c>
+      <c r="C32" t="s">
+        <v>264</v>
+      </c>
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
       <c r="F32" s="27"/>
       <c r="G32" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H32" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="2:12" ht="16.8" x14ac:dyDescent="0.3">
@@ -2411,376 +2417,372 @@
       <c r="E33" s="20"/>
       <c r="F33"/>
       <c r="G33" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H33" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C34" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D34" s="20">
         <v>3.367</v>
       </c>
       <c r="E34" s="41" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F34" s="27">
         <v>3.6549999999999998</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H34" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J34" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="D35" s="20">
         <v>3.5049999999999999</v>
       </c>
       <c r="E35" s="41" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F35" s="28">
         <v>4.33</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H35" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K35" s="36" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="D36" s="24"/>
       <c r="E36" s="41" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F36" s="27">
         <v>5.78</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H36" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I36" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J36" s="33"/>
       <c r="K36" s="8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C37" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="D37" s="20">
         <v>3.3140000000000001</v>
       </c>
       <c r="E37" s="41" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F37" s="28">
         <v>6.6349999999999998</v>
       </c>
       <c r="I37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J37" s="2"/>
       <c r="K37" s="8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="L37" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C38" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="D38" s="20"/>
       <c r="E38" s="41" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F38" s="27">
         <v>7.92</v>
       </c>
       <c r="K38" s="37" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="L38" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
     </row>
     <row r="39" spans="2:12" ht="16.2" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C39" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="41" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F39" s="27">
         <v>3.6549999999999998</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>54</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C40" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="D40" s="20"/>
       <c r="E40" s="41" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F40" s="27">
         <v>5.2549999999999999</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H40" t="s">
-        <v>162</v>
-      </c>
-      <c r="J40" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="K40" s="45"/>
+        <v>159</v>
+      </c>
+      <c r="I40" s="4"/>
+      <c r="J40" s="48"/>
+      <c r="K40" s="48"/>
+      <c r="L40" s="4"/>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C41" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D41" s="20"/>
       <c r="E41" s="41" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F41" s="27">
         <v>7.2750000000000004</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H41" t="s">
-        <v>163</v>
-      </c>
-      <c r="J41" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>177</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C42" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="41" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F42" s="27">
         <v>4.46</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H42" t="s">
-        <v>164</v>
-      </c>
-      <c r="J42" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>178</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C43" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="41" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F43" s="27">
         <v>4.3949999999999996</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H43" t="s">
-        <v>165</v>
-      </c>
-      <c r="J43" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>179</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="41" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F44" s="27">
         <v>2.19</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H44" t="s">
-        <v>166</v>
-      </c>
-      <c r="J44" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K44" s="7" t="s">
-        <v>180</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C45" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="41" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F45" s="27">
         <v>4.415</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H45" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C46" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="41" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F46" s="27">
         <v>2.92</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H46" t="s">
-        <v>168</v>
+        <v>261</v>
       </c>
       <c r="I46" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C47" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="41" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F47" s="27">
         <v>3.91</v>
       </c>
       <c r="I47" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C48" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="41" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F48" s="27">
         <v>4</v>
@@ -2788,39 +2790,49 @@
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C49" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="41" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F49" s="27">
         <v>4.7699999999999996</v>
       </c>
-      <c r="G49" s="36" t="s">
-        <v>80</v>
-      </c>
+      <c r="G49" s="36"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>262</v>
+      </c>
+      <c r="C50" t="s">
+        <v>263</v>
+      </c>
+      <c r="E50" s="4"/>
+      <c r="F50" s="49"/>
       <c r="G50" s="8"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B51" s="8"/>
       <c r="D51" s="4"/>
-      <c r="E51" s="1"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="49"/>
       <c r="G51" s="8"/>
       <c r="J51" s="2"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B52" s="8"/>
-      <c r="E52" s="1"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="49"/>
       <c r="J52" s="2"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B53" s="8"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="49"/>
     </row>
     <row r="58" spans="2:10" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B58" s="30"/>

</xml_diff>